<commit_message>
Added basic number postprocessing to jaffe2
</commit_message>
<xml_diff>
--- a/data/postprocessed/postprocessed_jaffe2_preAlexander.xlsx
+++ b/data/postprocessed/postprocessed_jaffe2_preAlexander.xlsx
@@ -529,8 +529,10 @@
           <t>Laterani</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>8434</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8434</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -1273,7 +1275,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8484 (600a</t>
+          <t>8484 (600</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1839,7 +1841,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1144 rebrv. 2.</t>
+          <t>1144 Febr. 2.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1871,7 +1873,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1144 rebrv. 2.</t>
+          <t>1144 Febr. 2.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -4337,7 +4339,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>8580 (6112a</t>
+          <t>8580 (6112</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -4647,7 +4649,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>1144 Rai. 1.</t>
+          <t>1144 Mai. 1.</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4679,7 +4681,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>1144 Rai. 1.</t>
+          <t>1144 Mai. 1.</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4707,7 +4709,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>1144 Rai. 4.</t>
+          <t>1144 Mai. 4.</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4739,7 +4741,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>1144 Rai. 4.</t>
+          <t>1144 Mai. 4.</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4771,7 +4773,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>1144 Rai. 4.</t>
+          <t>1144 Mai. 4.</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4803,7 +4805,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>1144 Rai. 4.</t>
+          <t>1144 Mai. 4.</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4835,7 +4837,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>1144 Rai. 10.</t>
+          <t>1144 Mai. 10.</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4867,7 +4869,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>1144 Rai. 10.</t>
+          <t>1144 Mai. 10.</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4899,7 +4901,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>1144 Rai. 10.</t>
+          <t>1144 Mai. 10.</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4931,7 +4933,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>1144 Rai. 10.</t>
+          <t>1144 Mai. 10.</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4959,7 +4961,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>1144 Rai. 11.</t>
+          <t>1144 Mai. 11.</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -5065,7 +5067,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>„ 8608</t>
+          <t xml:space="preserve"> 8608</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -5627,7 +5629,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>1144 lun. 1.</t>
+          <t>1144 Iun. 1.</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5659,7 +5661,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>1144 lun. 8.</t>
+          <t>1144 Iun. 8.</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -5907,7 +5909,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>1144 lul. 6.</t>
+          <t>1144 Iul. 6.</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -6749,7 +6751,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>8672 (6103a</t>
+          <t>8672 (6103</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -7611,7 +7613,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>1145 Lan. 1.</t>
+          <t>1145 Ian. 1.</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -7643,7 +7645,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>1145 Lan. 9.</t>
+          <t>1145 Ian. 9.</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -7675,7 +7677,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>1145 Lan. 11.</t>
+          <t>1145 Ian. 11.</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -7707,7 +7709,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>1145 Lan. 11.</t>
+          <t>1145 Ian. 11.</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -7739,7 +7741,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>1145 Lan. 11.</t>
+          <t>1145 Ian. 11.</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -7771,7 +7773,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>1145 Lan. 16.</t>
+          <t>1145 Ian. 16.</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -7803,7 +7805,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>1145 Lan. 16.</t>
+          <t>1145 Ian. 16.</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -7835,7 +7837,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>1145 Lan. 19.</t>
+          <t>1145 Ian. 19.</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -7867,7 +7869,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>1145 Lan. 20.</t>
+          <t>1145 Ian. 20.</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -7899,7 +7901,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>1145 Lan. 23.</t>
+          <t>1145 Ian. 23.</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -7931,7 +7933,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>1145 Lan. 31.</t>
+          <t>1145 Ian. 31.</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -7963,7 +7965,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>1145 Lan. 31.</t>
+          <t>1145 Ian. 31.</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -7995,7 +7997,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>171 Lan. 14.</t>
+          <t>171 Ian. 14.</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -8027,7 +8029,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>171 Lan. 14.</t>
+          <t>171 Ian. 14.</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -8297,7 +8299,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>„ 8719 (6184)</t>
+          <t xml:space="preserve"> 8719 (6184)</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
@@ -8361,7 +8363,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>p 8721</t>
+          <t xml:space="preserve"> 8721</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -9235,7 +9237,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>1145 Nai. 30.</t>
+          <t>1145 Mai. 30.</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -9267,7 +9269,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>1145 Nai. 30.</t>
+          <t>1145 Mai. 30.</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -9299,7 +9301,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>1145 Nai. 8.</t>
+          <t>1145 Mai. 8.</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -9331,7 +9333,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>1145 Nai. 8.</t>
+          <t>1145 Mai. 8.</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -9939,7 +9941,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>1145 Lan. 28.</t>
+          <t>1145 Ian. 28.</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11829,7 +11831,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>s834 (6195)</t>
+          <t>834 (6195)</t>
         </is>
       </c>
       <c r="E362" t="inlineStr">
@@ -11851,7 +11853,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>1146 lan. 2.</t>
+          <t>1146 Ian. 2.</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
@@ -11883,7 +11885,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>1146 lan. 3.</t>
+          <t>1146 Ian. 3.</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -11915,7 +11917,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>1146 lan. 1.</t>
+          <t>1146 Ian. 1.</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
@@ -11947,7 +11949,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>1146 lan. 7.</t>
+          <t>1146 Ian. 7.</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
@@ -11979,7 +11981,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>1146 lan. 8.</t>
+          <t>1146 Ian. 8.</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -12011,7 +12013,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>1146 lan. 9.</t>
+          <t>1146 Ian. 9.</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
@@ -12043,7 +12045,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>1146 lan. 10.</t>
+          <t>1146 Ian. 10.</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
@@ -12075,7 +12077,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>1146 lan. 12.</t>
+          <t>1146 Ian. 12.</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
@@ -12107,7 +12109,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>1146 lan. 15.</t>
+          <t>1146 Ian. 15.</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
@@ -12139,7 +12141,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>1146 lan. 16.</t>
+          <t>1146 Ian. 16.</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
@@ -12171,7 +12173,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>1146 lan. 17.</t>
+          <t>1146 Ian. 17.</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
@@ -12203,7 +12205,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>1146 lan. 19.</t>
+          <t>1146 Ian. 19.</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
@@ -12235,7 +12237,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>1146 lan. 19.</t>
+          <t>1146 Ian. 19.</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
@@ -12267,7 +12269,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>1146 lan. 21.</t>
+          <t>1146 Ian. 21.</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
@@ -12299,7 +12301,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>1146 lan. 21.</t>
+          <t>1146 Ian. 21.</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
@@ -12331,7 +12333,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>1146 lan. 29.</t>
+          <t>1146 Ian. 29.</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -12363,7 +12365,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>1146 lan. 30.</t>
+          <t>1146 Ian. 30.</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -12395,7 +12397,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>854 lan. 5.</t>
+          <t>854 Ian. 5.</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
@@ -12427,7 +12429,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>854 lan. 9.</t>
+          <t>854 Ian. 9.</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -12459,7 +12461,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>854 lan. 11.</t>
+          <t>854 Ian. 11.</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
@@ -12501,7 +12503,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>p 8858</t>
+          <t xml:space="preserve"> 8858</t>
         </is>
       </c>
       <c r="E383" t="inlineStr">
@@ -14401,7 +14403,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>. 1146.</t>
+          <t xml:space="preserve"> 1146</t>
         </is>
       </c>
       <c r="E443" t="inlineStr">
@@ -14615,7 +14617,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>1146 lan. 2.</t>
+          <t>1146 Ian. 2.</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
@@ -14647,7 +14649,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>1146 lan. 6.</t>
+          <t>1146 Ian. 6.</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
@@ -14679,7 +14681,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>1146 lan. 12.</t>
+          <t>1146 Ian. 12.</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
@@ -14711,7 +14713,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>1146 lan. 14.</t>
+          <t>1146 Ian. 14.</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
@@ -14743,7 +14745,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>1146 lan. 14.</t>
+          <t>1146 Ian. 14.</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
@@ -14775,7 +14777,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>1146 lan. 14.</t>
+          <t>1146 Ian. 14.</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
@@ -15485,7 +15487,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>8958 (6261a</t>
+          <t>8958 (6261</t>
         </is>
       </c>
       <c r="E477" t="inlineStr">
@@ -16769,7 +16771,7 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>8998 (6285a</t>
+          <t>8998 (6285</t>
         </is>
       </c>
       <c r="E518" t="inlineStr">
@@ -16847,7 +16849,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>1147 lan. 7.</t>
+          <t>1147 Ian. 7.</t>
         </is>
       </c>
       <c r="C521" t="inlineStr">
@@ -16879,7 +16881,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>1147 lan. 7.</t>
+          <t>1147 Ian. 7.</t>
         </is>
       </c>
       <c r="C522" t="inlineStr">
@@ -16911,7 +16913,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>1147 lan. 7.</t>
+          <t>1147 Ian. 7.</t>
         </is>
       </c>
       <c r="C523" t="inlineStr">
@@ -16975,7 +16977,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>1147 lan. 11.</t>
+          <t>1147 Ian. 11.</t>
         </is>
       </c>
       <c r="C525" t="inlineStr">
@@ -17113,7 +17115,7 @@
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>9009.</t>
+          <t>9009</t>
         </is>
       </c>
       <c r="E529" t="inlineStr">
@@ -19361,7 +19363,7 @@
       </c>
       <c r="D601" t="inlineStr">
         <is>
-          <t>9072 (6321a</t>
+          <t>9072 (6321</t>
         </is>
       </c>
       <c r="E601" t="inlineStr">
@@ -19393,7 +19395,7 @@
       </c>
       <c r="D602" t="inlineStr">
         <is>
-          <t>9073 (6521“</t>
+          <t>9073 (6521</t>
         </is>
       </c>
       <c r="E602" t="inlineStr">
@@ -19415,7 +19417,7 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>1147 Lun. 5.</t>
+          <t>1147 Iun. 5.</t>
         </is>
       </c>
       <c r="C603" t="inlineStr">
@@ -19447,7 +19449,7 @@
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>1147 Lun. 5.</t>
+          <t>1147 Iun. 5.</t>
         </is>
       </c>
       <c r="C604" t="inlineStr">
@@ -19479,7 +19481,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>1147 Lun. 7.</t>
+          <t>1147 Iun. 7.</t>
         </is>
       </c>
       <c r="C605" t="inlineStr">
@@ -19571,7 +19573,7 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>1147 Arr. 11.</t>
+          <t>1147 Apr. 11.</t>
         </is>
       </c>
       <c r="C608" t="inlineStr">
@@ -19595,7 +19597,7 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>1147 Arr. 12.</t>
+          <t>1147 Apr. 12.</t>
         </is>
       </c>
       <c r="C609" t="inlineStr">
@@ -19619,7 +19621,7 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>1147 Arr. 13.</t>
+          <t>1147 Apr. 13.</t>
         </is>
       </c>
       <c r="C610" t="inlineStr">
@@ -19651,7 +19653,7 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>1147 Arr. 14.</t>
+          <t>1147 Apr. 14.</t>
         </is>
       </c>
       <c r="C611" t="inlineStr">
@@ -19683,7 +19685,7 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>1147 Arr. 14.</t>
+          <t>1147 Apr. 14.</t>
         </is>
       </c>
       <c r="C612" t="inlineStr">
@@ -19715,7 +19717,7 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>1147 Arr. 17.</t>
+          <t>1147 Apr. 17.</t>
         </is>
       </c>
       <c r="C613" t="inlineStr">
@@ -19747,7 +19749,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>1147 Arr. 15.</t>
+          <t>1147 Apr. 15.</t>
         </is>
       </c>
       <c r="C614" t="inlineStr">
@@ -19905,7 +19907,7 @@
       </c>
       <c r="D619" t="inlineStr">
         <is>
-          <t>9086 (6376a</t>
+          <t>9086 (6376</t>
         </is>
       </c>
       <c r="E619" t="inlineStr">
@@ -19927,7 +19929,7 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>1147 lun. 21.</t>
+          <t>1147 Iun. 21.</t>
         </is>
       </c>
       <c r="C620" t="inlineStr">
@@ -19959,7 +19961,7 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>1147 lun. 26.</t>
+          <t>1147 Iun. 26.</t>
         </is>
       </c>
       <c r="C621" t="inlineStr">
@@ -19991,7 +19993,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>1147 lun. 26.</t>
+          <t>1147 Iun. 26.</t>
         </is>
       </c>
       <c r="C622" t="inlineStr">
@@ -20023,7 +20025,7 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>1147 lun. 29.</t>
+          <t>1147 Iun. 29.</t>
         </is>
       </c>
       <c r="C623" t="inlineStr">
@@ -20055,7 +20057,7 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>1147 lun. 30.</t>
+          <t>1147 Iun. 30.</t>
         </is>
       </c>
       <c r="C624" t="inlineStr">
@@ -20087,7 +20089,7 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>1147 lun. 30.</t>
+          <t>1147 Iun. 30.</t>
         </is>
       </c>
       <c r="C625" t="inlineStr">
@@ -21351,7 +21353,7 @@
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t xml:space="preserve">1147 Septeanr.  </t>
+          <t xml:space="preserve">1147 Sept.  </t>
         </is>
       </c>
       <c r="C665" t="inlineStr">
@@ -21667,7 +21669,7 @@
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t xml:space="preserve">140 lulOct.  </t>
+          <t xml:space="preserve">140 Oct.  </t>
         </is>
       </c>
       <c r="C675" t="inlineStr">
@@ -21677,7 +21679,7 @@
       </c>
       <c r="D675" t="inlineStr">
         <is>
-          <t>9143a</t>
+          <t>9143</t>
         </is>
       </c>
       <c r="E675" t="inlineStr">
@@ -22947,7 +22949,7 @@
       </c>
       <c r="B720" t="inlineStr">
         <is>
-          <t>1148 Lan. 13.</t>
+          <t>1148 Ian. 13.</t>
         </is>
       </c>
       <c r="C720" t="inlineStr">
@@ -22975,7 +22977,7 @@
       </c>
       <c r="B721" t="inlineStr">
         <is>
-          <t>1148 Lan. 20.</t>
+          <t>1148 Ian. 20.</t>
         </is>
       </c>
       <c r="C721" t="inlineStr">
@@ -23007,7 +23009,7 @@
       </c>
       <c r="B722" t="inlineStr">
         <is>
-          <t>1148 Lan. 20.</t>
+          <t>1148 Ian. 20.</t>
         </is>
       </c>
       <c r="C722" t="inlineStr">
@@ -23039,7 +23041,7 @@
       </c>
       <c r="B723" t="inlineStr">
         <is>
-          <t>1148 Lan. 20.</t>
+          <t>1148 Ian. 20.</t>
         </is>
       </c>
       <c r="C723" t="inlineStr">
@@ -23071,7 +23073,7 @@
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>1148 Lan. 27.</t>
+          <t>1148 Ian. 27.</t>
         </is>
       </c>
       <c r="C724" t="inlineStr">
@@ -23103,7 +23105,7 @@
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>1148 Lan. 28.</t>
+          <t>1148 Ian. 28.</t>
         </is>
       </c>
       <c r="C725" t="inlineStr">
@@ -23135,7 +23137,7 @@
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>1148 Lan. 28.</t>
+          <t>1148 Ian. 28.</t>
         </is>
       </c>
       <c r="C726" t="inlineStr">
@@ -23167,7 +23169,7 @@
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>1148 Lan. 28.</t>
+          <t>1148 Ian. 28.</t>
         </is>
       </c>
       <c r="C727" t="inlineStr">
@@ -23199,7 +23201,7 @@
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>1148 Lan. 31.</t>
+          <t>1148 Ian. 31.</t>
         </is>
       </c>
       <c r="C728" t="inlineStr">
@@ -23425,7 +23427,7 @@
       </c>
       <c r="D735" t="inlineStr">
         <is>
-          <t>„ 9187 (6386)</t>
+          <t xml:space="preserve"> 9187 (6386)</t>
         </is>
       </c>
       <c r="E735" t="inlineStr">
@@ -25651,7 +25653,7 @@
       </c>
       <c r="B806" t="inlineStr">
         <is>
-          <t>1148 lul. 7.</t>
+          <t>1148 Iul. 7.</t>
         </is>
       </c>
       <c r="C806" t="inlineStr">
@@ -25715,7 +25717,7 @@
       </c>
       <c r="B808" t="inlineStr">
         <is>
-          <t>1148 lul. 7.</t>
+          <t>1148 Iul. 7.</t>
         </is>
       </c>
       <c r="C808" t="inlineStr">
@@ -25747,7 +25749,7 @@
       </c>
       <c r="B809" t="inlineStr">
         <is>
-          <t>1148 lul. 7.</t>
+          <t>1148 Iul. 7.</t>
         </is>
       </c>
       <c r="C809" t="inlineStr">
@@ -25807,7 +25809,7 @@
       </c>
       <c r="B811" t="inlineStr">
         <is>
-          <t>1148 lul. 9.</t>
+          <t>1148 Iul. 9.</t>
         </is>
       </c>
       <c r="C811" t="inlineStr">
@@ -25831,7 +25833,7 @@
       </c>
       <c r="B812" t="inlineStr">
         <is>
-          <t>1148 lul. 15.</t>
+          <t>1148 Iul. 15.</t>
         </is>
       </c>
       <c r="C812" t="inlineStr">
@@ -25863,7 +25865,7 @@
       </c>
       <c r="B813" t="inlineStr">
         <is>
-          <t>1148 lul. 16.</t>
+          <t>1148 Iul. 16.</t>
         </is>
       </c>
       <c r="C813" t="inlineStr">
@@ -25895,7 +25897,7 @@
       </c>
       <c r="B814" t="inlineStr">
         <is>
-          <t>1148 lul. 21.</t>
+          <t>1148 Iul. 21.</t>
         </is>
       </c>
       <c r="C814" t="inlineStr">
@@ -25927,7 +25929,7 @@
       </c>
       <c r="B815" t="inlineStr">
         <is>
-          <t>1148 lul. 22.</t>
+          <t>1148 Iul. 22.</t>
         </is>
       </c>
       <c r="C815" t="inlineStr">
@@ -25959,7 +25961,7 @@
       </c>
       <c r="B816" t="inlineStr">
         <is>
-          <t>1148 lul. 22.</t>
+          <t>1148 Iul. 22.</t>
         </is>
       </c>
       <c r="C816" t="inlineStr">
@@ -25991,7 +25993,7 @@
       </c>
       <c r="B817" t="inlineStr">
         <is>
-          <t>1148 lul. 29.</t>
+          <t>1148 Iul. 29.</t>
         </is>
       </c>
       <c r="C817" t="inlineStr">
@@ -26899,7 +26901,7 @@
       </c>
       <c r="B847" t="inlineStr">
         <is>
-          <t>1148 Bec. 90.</t>
+          <t>1148 Dec. 90.</t>
         </is>
       </c>
       <c r="C847" t="inlineStr">
@@ -27115,7 +27117,7 @@
       </c>
       <c r="B854" t="inlineStr">
         <is>
-          <t>1149 Lan. 1.</t>
+          <t>1149 Ian. 1.</t>
         </is>
       </c>
       <c r="C854" t="inlineStr">
@@ -27147,7 +27149,7 @@
       </c>
       <c r="B855" t="inlineStr">
         <is>
-          <t>1149 Lan. 2.</t>
+          <t>1149 Ian. 2.</t>
         </is>
       </c>
       <c r="C855" t="inlineStr">
@@ -27179,7 +27181,7 @@
       </c>
       <c r="B856" t="inlineStr">
         <is>
-          <t>1149 Lan. 15.</t>
+          <t>1149 Ian. 15.</t>
         </is>
       </c>
       <c r="C856" t="inlineStr">
@@ -27211,7 +27213,7 @@
       </c>
       <c r="B857" t="inlineStr">
         <is>
-          <t>1149 Lan. 18.</t>
+          <t>1149 Ian. 18.</t>
         </is>
       </c>
       <c r="C857" t="inlineStr">
@@ -27243,7 +27245,7 @@
       </c>
       <c r="B858" t="inlineStr">
         <is>
-          <t>1149 Lan. 28.</t>
+          <t>1149 Ian. 28.</t>
         </is>
       </c>
       <c r="C858" t="inlineStr">
@@ -27253,7 +27255,7 @@
       </c>
       <c r="D858" t="inlineStr">
         <is>
-          <t>f9320</t>
+          <t>9320</t>
         </is>
       </c>
       <c r="E858" t="inlineStr">
@@ -27275,7 +27277,7 @@
       </c>
       <c r="B859" t="inlineStr">
         <is>
-          <t>1149 Lan. 31.</t>
+          <t>1149 Ian. 31.</t>
         </is>
       </c>
       <c r="C859" t="inlineStr">
@@ -27637,7 +27639,7 @@
       </c>
       <c r="D870" t="inlineStr">
         <is>
-          <t>p9332 (6480)</t>
+          <t>9332 (6480)</t>
         </is>
       </c>
       <c r="E870" t="inlineStr">
@@ -27861,7 +27863,7 @@
       </c>
       <c r="D877" t="inlineStr">
         <is>
-          <t>9339 (6483a</t>
+          <t>9339 (6483</t>
         </is>
       </c>
       <c r="E877" t="inlineStr">
@@ -27979,7 +27981,7 @@
       </c>
       <c r="B881" t="inlineStr">
         <is>
-          <t>1149 Lan. 14.</t>
+          <t>1149 Ian. 14.</t>
         </is>
       </c>
       <c r="C881" t="inlineStr">
@@ -28011,7 +28013,7 @@
       </c>
       <c r="B882" t="inlineStr">
         <is>
-          <t>1149 Lan. 23.</t>
+          <t>1149 Ian. 23.</t>
         </is>
       </c>
       <c r="C882" t="inlineStr">
@@ -28803,7 +28805,7 @@
       </c>
       <c r="B907" t="inlineStr">
         <is>
-          <t>1150 lan. 23.</t>
+          <t>1150 Ian. 23.</t>
         </is>
       </c>
       <c r="C907" t="inlineStr">
@@ -28835,7 +28837,7 @@
       </c>
       <c r="B908" t="inlineStr">
         <is>
-          <t>1150 lan. 30.</t>
+          <t>1150 Ian. 30.</t>
         </is>
       </c>
       <c r="C908" t="inlineStr">
@@ -29535,7 +29537,7 @@
       </c>
       <c r="B930" t="inlineStr">
         <is>
-          <t>1150 lun. 5.</t>
+          <t>1150 Iun. 5.</t>
         </is>
       </c>
       <c r="C930" t="inlineStr">
@@ -29567,7 +29569,7 @@
       </c>
       <c r="B931" t="inlineStr">
         <is>
-          <t>1150 lun. 10.</t>
+          <t>1150 Iun. 10.</t>
         </is>
       </c>
       <c r="C931" t="inlineStr">
@@ -29599,7 +29601,7 @@
       </c>
       <c r="B932" t="inlineStr">
         <is>
-          <t>1150 lun. 12.</t>
+          <t>1150 Iun. 12.</t>
         </is>
       </c>
       <c r="C932" t="inlineStr">
@@ -29631,7 +29633,7 @@
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>1150 lun. 15.</t>
+          <t>1150 Iun. 15.</t>
         </is>
       </c>
       <c r="C933" t="inlineStr">
@@ -29663,7 +29665,7 @@
       </c>
       <c r="B934" t="inlineStr">
         <is>
-          <t>1150 lun. 19.</t>
+          <t>1150 Iun. 19.</t>
         </is>
       </c>
       <c r="C934" t="inlineStr">
@@ -29695,7 +29697,7 @@
       </c>
       <c r="B935" t="inlineStr">
         <is>
-          <t>1150 lun. 22.</t>
+          <t>1150 Iun. 22.</t>
         </is>
       </c>
       <c r="C935" t="inlineStr">
@@ -29727,7 +29729,7 @@
       </c>
       <c r="B936" t="inlineStr">
         <is>
-          <t>1150 lun. 24.</t>
+          <t>1150 Iun. 24.</t>
         </is>
       </c>
       <c r="C936" t="inlineStr">
@@ -30127,7 +30129,7 @@
       </c>
       <c r="B949" t="inlineStr">
         <is>
-          <t>1150 Nor. 21.</t>
+          <t>1150 Nov. 21.</t>
         </is>
       </c>
       <c r="C949" t="inlineStr">
@@ -30159,7 +30161,7 @@
       </c>
       <c r="B950" t="inlineStr">
         <is>
-          <t>1150 Nor. 21.</t>
+          <t>1150 Nov. 21.</t>
         </is>
       </c>
       <c r="C950" t="inlineStr">
@@ -30201,7 +30203,7 @@
       </c>
       <c r="D951" t="inlineStr">
         <is>
-          <t>9412a</t>
+          <t>9412</t>
         </is>
       </c>
       <c r="E951" t="inlineStr">
@@ -30223,7 +30225,7 @@
       </c>
       <c r="B952" t="inlineStr">
         <is>
-          <t>1150 Nor. 21.</t>
+          <t>1150 Nov. 21.</t>
         </is>
       </c>
       <c r="C952" t="inlineStr">
@@ -31127,7 +31129,7 @@
       </c>
       <c r="B981" t="inlineStr">
         <is>
-          <t>1151 lan. 15.</t>
+          <t>1151 Ian. 15.</t>
         </is>
       </c>
       <c r="C981" t="inlineStr">
@@ -31159,7 +31161,7 @@
       </c>
       <c r="B982" t="inlineStr">
         <is>
-          <t>1151 lan. 13.</t>
+          <t>1151 Ian. 13.</t>
         </is>
       </c>
       <c r="C982" t="inlineStr">
@@ -31191,7 +31193,7 @@
       </c>
       <c r="B983" t="inlineStr">
         <is>
-          <t>1151 lan. 21.</t>
+          <t>1151 Ian. 21.</t>
         </is>
       </c>
       <c r="C983" t="inlineStr">
@@ -31223,7 +31225,7 @@
       </c>
       <c r="B984" t="inlineStr">
         <is>
-          <t>1151 lan. 24.</t>
+          <t>1151 Ian. 24.</t>
         </is>
       </c>
       <c r="C984" t="inlineStr">
@@ -31255,7 +31257,7 @@
       </c>
       <c r="B985" t="inlineStr">
         <is>
-          <t>1151 lan. 36.</t>
+          <t>1151 Ian. 36.</t>
         </is>
       </c>
       <c r="C985" t="inlineStr">
@@ -31287,7 +31289,7 @@
       </c>
       <c r="B986" t="inlineStr">
         <is>
-          <t>1151 lan. 26.</t>
+          <t>1151 Ian. 26.</t>
         </is>
       </c>
       <c r="C986" t="inlineStr">
@@ -32615,7 +32617,7 @@
       </c>
       <c r="B1028" t="inlineStr">
         <is>
-          <t>1151 lun. 6.</t>
+          <t>1151 Iun. 6.</t>
         </is>
       </c>
       <c r="C1028" t="inlineStr">
@@ -32647,7 +32649,7 @@
       </c>
       <c r="B1029" t="inlineStr">
         <is>
-          <t>1151 lun. 6.</t>
+          <t>1151 Iun. 6.</t>
         </is>
       </c>
       <c r="C1029" t="inlineStr">
@@ -32679,7 +32681,7 @@
       </c>
       <c r="B1030" t="inlineStr">
         <is>
-          <t>1151 lun. 13.</t>
+          <t>1151 Iun. 13.</t>
         </is>
       </c>
       <c r="C1030" t="inlineStr">
@@ -32711,7 +32713,7 @@
       </c>
       <c r="B1031" t="inlineStr">
         <is>
-          <t>1151 lun. 22.</t>
+          <t>1151 Iun. 22.</t>
         </is>
       </c>
       <c r="C1031" t="inlineStr">
@@ -32807,7 +32809,7 @@
       </c>
       <c r="B1034" t="inlineStr">
         <is>
-          <t>1151 lul. 10.</t>
+          <t>1151 Iul. 10.</t>
         </is>
       </c>
       <c r="C1034" t="inlineStr">
@@ -33547,7 +33549,7 @@
       </c>
       <c r="B1058" t="inlineStr">
         <is>
-          <t>1152 Lan. 8.</t>
+          <t>1152 Ian. 8.</t>
         </is>
       </c>
       <c r="C1058" t="inlineStr">
@@ -33579,7 +33581,7 @@
       </c>
       <c r="B1059" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1059" t="inlineStr">
@@ -33611,7 +33613,7 @@
       </c>
       <c r="B1060" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1060" t="inlineStr">
@@ -33643,7 +33645,7 @@
       </c>
       <c r="B1061" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1061" t="inlineStr">
@@ -33675,7 +33677,7 @@
       </c>
       <c r="B1062" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1062" t="inlineStr">
@@ -33707,7 +33709,7 @@
       </c>
       <c r="B1063" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1063" t="inlineStr">
@@ -33735,7 +33737,7 @@
       </c>
       <c r="B1064" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1064" t="inlineStr">
@@ -33767,7 +33769,7 @@
       </c>
       <c r="B1065" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1065" t="inlineStr">
@@ -33799,7 +33801,7 @@
       </c>
       <c r="B1066" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1066" t="inlineStr">
@@ -33831,7 +33833,7 @@
       </c>
       <c r="B1067" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1067" t="inlineStr">
@@ -33863,7 +33865,7 @@
       </c>
       <c r="B1068" t="inlineStr">
         <is>
-          <t>1152 Lan. 9.</t>
+          <t>1152 Ian. 9.</t>
         </is>
       </c>
       <c r="C1068" t="inlineStr">
@@ -34399,7 +34401,7 @@
       </c>
       <c r="B1085" t="inlineStr">
         <is>
-          <t>1152 lan. 28.</t>
+          <t>1152 Ian. 28.</t>
         </is>
       </c>
       <c r="C1085" t="inlineStr">
@@ -34431,7 +34433,7 @@
       </c>
       <c r="B1086" t="inlineStr">
         <is>
-          <t>1152 lan. 29.</t>
+          <t>1152 Ian. 29.</t>
         </is>
       </c>
       <c r="C1086" t="inlineStr">
@@ -35135,7 +35137,7 @@
       </c>
       <c r="B1108" t="inlineStr">
         <is>
-          <t>1152 Api. 5.</t>
+          <t>1152 Apr. 5.</t>
         </is>
       </c>
       <c r="C1108" t="inlineStr">
@@ -35167,7 +35169,7 @@
       </c>
       <c r="B1109" t="inlineStr">
         <is>
-          <t>1152 Api. 7.</t>
+          <t>1152 Apr. 7.</t>
         </is>
       </c>
       <c r="C1109" t="inlineStr">
@@ -35199,7 +35201,7 @@
       </c>
       <c r="B1110" t="inlineStr">
         <is>
-          <t>1152 Api. 8.</t>
+          <t>1152 Apr. 8.</t>
         </is>
       </c>
       <c r="C1110" t="inlineStr">
@@ -35231,7 +35233,7 @@
       </c>
       <c r="B1111" t="inlineStr">
         <is>
-          <t>1152 Api. 15.</t>
+          <t>1152 Apr. 15.</t>
         </is>
       </c>
       <c r="C1111" t="inlineStr">
@@ -35831,7 +35833,7 @@
       </c>
       <c r="B1130" t="inlineStr">
         <is>
-          <t>1152 lun. 4.</t>
+          <t>1152 Iun. 4.</t>
         </is>
       </c>
       <c r="C1130" t="inlineStr">
@@ -35863,7 +35865,7 @@
       </c>
       <c r="B1131" t="inlineStr">
         <is>
-          <t>1152 lun. 9.</t>
+          <t>1152 Iun. 9.</t>
         </is>
       </c>
       <c r="C1131" t="inlineStr">
@@ -35895,7 +35897,7 @@
       </c>
       <c r="B1132" t="inlineStr">
         <is>
-          <t>1152 lun. 15.</t>
+          <t>1152 Iun. 15.</t>
         </is>
       </c>
       <c r="C1132" t="inlineStr">
@@ -35927,7 +35929,7 @@
       </c>
       <c r="B1133" t="inlineStr">
         <is>
-          <t>1152 lun. 15.</t>
+          <t>1152 Iun. 15.</t>
         </is>
       </c>
       <c r="C1133" t="inlineStr">
@@ -36471,7 +36473,7 @@
       </c>
       <c r="B1150" t="inlineStr">
         <is>
-          <t>1152 Oet. 1.</t>
+          <t>1152 Oct. 1.</t>
         </is>
       </c>
       <c r="C1150" t="inlineStr">
@@ -36503,7 +36505,7 @@
       </c>
       <c r="B1151" t="inlineStr">
         <is>
-          <t>1152 Oet. 9.</t>
+          <t>1152 Oct. 9.</t>
         </is>
       </c>
       <c r="C1151" t="inlineStr">
@@ -36527,7 +36529,7 @@
       </c>
       <c r="B1152" t="inlineStr">
         <is>
-          <t>1152 Oet. 19.</t>
+          <t>1152 Oct. 19.</t>
         </is>
       </c>
       <c r="C1152" t="inlineStr">
@@ -36559,7 +36561,7 @@
       </c>
       <c r="B1153" t="inlineStr">
         <is>
-          <t>1152 Oet. 23.</t>
+          <t>1152 Oct. 23.</t>
         </is>
       </c>
       <c r="C1153" t="inlineStr">
@@ -37549,7 +37551,7 @@
       </c>
       <c r="D1184" t="inlineStr">
         <is>
-          <t>p9640</t>
+          <t>9640</t>
         </is>
       </c>
       <c r="E1184" t="inlineStr">
@@ -37855,7 +37857,7 @@
       </c>
       <c r="B1194" t="inlineStr">
         <is>
-          <t>1146 lan. 115317.</t>
+          <t>1146 Ian. 115317.</t>
         </is>
       </c>
       <c r="C1194" t="inlineStr">
@@ -37887,7 +37889,7 @@
       </c>
       <c r="B1195" t="inlineStr">
         <is>
-          <t>1146 lan. 115323.</t>
+          <t>1146 Ian. 115323.</t>
         </is>
       </c>
       <c r="C1195" t="inlineStr">
@@ -38047,7 +38049,7 @@
       </c>
       <c r="B1200" t="inlineStr">
         <is>
-          <t>1150 lan. 115316.</t>
+          <t>1150 Ian. 115316.</t>
         </is>
       </c>
       <c r="C1200" t="inlineStr">
@@ -38079,7 +38081,7 @@
       </c>
       <c r="B1201" t="inlineStr">
         <is>
-          <t>1150 lan. 115324.</t>
+          <t>1150 Ian. 115324.</t>
         </is>
       </c>
       <c r="C1201" t="inlineStr">
@@ -38305,7 +38307,7 @@
       </c>
       <c r="D1208" t="inlineStr">
         <is>
-          <t>1153.</t>
+          <t>1153</t>
         </is>
       </c>
       <c r="E1208" t="inlineStr">
@@ -39435,7 +39437,7 @@
       </c>
       <c r="B1244" t="inlineStr">
         <is>
-          <t>1153 Ran. 3.</t>
+          <t>1153 Ian. 3.</t>
         </is>
       </c>
       <c r="C1244" t="inlineStr">
@@ -39463,7 +39465,7 @@
       </c>
       <c r="B1245" t="inlineStr">
         <is>
-          <t>1153 Ran. 3.</t>
+          <t>1153 Ian. 3.</t>
         </is>
       </c>
       <c r="C1245" t="inlineStr">
@@ -39495,7 +39497,7 @@
       </c>
       <c r="B1246" t="inlineStr">
         <is>
-          <t>1153 Ran. 14.</t>
+          <t>1153 Ian. 14.</t>
         </is>
       </c>
       <c r="C1246" t="inlineStr">
@@ -39559,7 +39561,7 @@
       </c>
       <c r="B1248" t="inlineStr">
         <is>
-          <t>1153 Ran. 10.</t>
+          <t>1153 Ian. 10.</t>
         </is>
       </c>
       <c r="C1248" t="inlineStr">
@@ -39655,7 +39657,7 @@
       </c>
       <c r="B1251" t="inlineStr">
         <is>
-          <t>1153 Ran. 3.</t>
+          <t>1153 Ian. 3.</t>
         </is>
       </c>
       <c r="C1251" t="inlineStr">
@@ -39687,7 +39689,7 @@
       </c>
       <c r="B1252" t="inlineStr">
         <is>
-          <t>1153 Ran. 4.</t>
+          <t>1153 Ian. 4.</t>
         </is>
       </c>
       <c r="C1252" t="inlineStr">
@@ -39719,7 +39721,7 @@
       </c>
       <c r="B1253" t="inlineStr">
         <is>
-          <t>1153 Ran. 12.</t>
+          <t>1153 Ian. 12.</t>
         </is>
       </c>
       <c r="C1253" t="inlineStr">
@@ -39751,7 +39753,7 @@
       </c>
       <c r="B1254" t="inlineStr">
         <is>
-          <t>1153 Ran. 12.</t>
+          <t>1153 Ian. 12.</t>
         </is>
       </c>
       <c r="C1254" t="inlineStr">
@@ -39783,7 +39785,7 @@
       </c>
       <c r="B1255" t="inlineStr">
         <is>
-          <t xml:space="preserve">1153 Ran.  </t>
+          <t xml:space="preserve">1153 Ian.  </t>
         </is>
       </c>
       <c r="C1255" t="inlineStr">
@@ -39815,7 +39817,7 @@
       </c>
       <c r="B1256" t="inlineStr">
         <is>
-          <t>1153 Ran. 16.</t>
+          <t>1153 Ian. 16.</t>
         </is>
       </c>
       <c r="C1256" t="inlineStr">
@@ -39843,7 +39845,7 @@
       </c>
       <c r="B1257" t="inlineStr">
         <is>
-          <t>1153 Ran. 16.</t>
+          <t>1153 Ian. 16.</t>
         </is>
       </c>
       <c r="C1257" t="inlineStr">
@@ -39875,7 +39877,7 @@
       </c>
       <c r="B1258" t="inlineStr">
         <is>
-          <t>1153 Ran. 16.</t>
+          <t>1153 Ian. 16.</t>
         </is>
       </c>
       <c r="C1258" t="inlineStr">
@@ -39999,7 +40001,7 @@
       </c>
       <c r="B1262" t="inlineStr">
         <is>
-          <t>1153 Lun. 7.</t>
+          <t>1153 Iun. 7.</t>
         </is>
       </c>
       <c r="C1262" t="inlineStr">
@@ -40031,7 +40033,7 @@
       </c>
       <c r="B1263" t="inlineStr">
         <is>
-          <t>1153 Lun. 13.</t>
+          <t>1153 Iun. 13.</t>
         </is>
       </c>
       <c r="C1263" t="inlineStr">
@@ -40063,7 +40065,7 @@
       </c>
       <c r="B1264" t="inlineStr">
         <is>
-          <t>1153 Lun. 16.</t>
+          <t>1153 Iun. 16.</t>
         </is>
       </c>
       <c r="C1264" t="inlineStr">
@@ -40095,7 +40097,7 @@
       </c>
       <c r="B1265" t="inlineStr">
         <is>
-          <t>1153 Lun. 20.</t>
+          <t>1153 Iun. 20.</t>
         </is>
       </c>
       <c r="C1265" t="inlineStr">
@@ -40127,7 +40129,7 @@
       </c>
       <c r="B1266" t="inlineStr">
         <is>
-          <t>1153 Lun. 28.</t>
+          <t>1153 Iun. 28.</t>
         </is>
       </c>
       <c r="C1266" t="inlineStr">
@@ -40159,7 +40161,7 @@
       </c>
       <c r="B1267" t="inlineStr">
         <is>
-          <t>1153 Lun. 29.</t>
+          <t>1153 Iun. 29.</t>
         </is>
       </c>
       <c r="C1267" t="inlineStr">
@@ -40191,7 +40193,7 @@
       </c>
       <c r="B1268" t="inlineStr">
         <is>
-          <t>1153 Lun. 29.</t>
+          <t>1153 Iun. 29.</t>
         </is>
       </c>
       <c r="C1268" t="inlineStr">
@@ -40407,11 +40409,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D1275" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
+      <c r="D1275" t="inlineStr"/>
       <c r="E1275" t="inlineStr">
         <is>
           <t>„7 40 Monasterii S. Nicolai Brunwillarensis possessiones confirmat, petente Geldolpho abbate. („Dat. Romae, 3 non. Sept., anno nostro I“.) Chron. Brunwylr. in Annal. d. hist. Ver. f. d. Niederrhcin XVII. 147, (Pertz Archiv XII. 130).</t>
@@ -40601,7 +40599,7 @@
       </c>
       <c r="D1281" t="inlineStr">
         <is>
-          <t>„716</t>
+          <t>716</t>
         </is>
       </c>
       <c r="E1281" t="inlineStr">
@@ -40633,7 +40631,7 @@
       </c>
       <c r="D1282" t="inlineStr">
         <is>
-          <t>251*</t>
+          <t>251</t>
         </is>
       </c>
       <c r="E1282" t="inlineStr">
@@ -41103,7 +41101,7 @@
       </c>
       <c r="B1297" t="inlineStr">
         <is>
-          <t>1153 Dcc. 3.</t>
+          <t>1153 Dec. 3.</t>
         </is>
       </c>
       <c r="C1297" t="inlineStr">
@@ -41135,7 +41133,7 @@
       </c>
       <c r="B1298" t="inlineStr">
         <is>
-          <t>1153 Dcc. 6.</t>
+          <t>1153 Dec. 6.</t>
         </is>
       </c>
       <c r="C1298" t="inlineStr">
@@ -41167,7 +41165,7 @@
       </c>
       <c r="B1299" t="inlineStr">
         <is>
-          <t>1153 Dcc. 6.</t>
+          <t>1153 Dec. 6.</t>
         </is>
       </c>
       <c r="C1299" t="inlineStr">
@@ -41199,7 +41197,7 @@
       </c>
       <c r="B1300" t="inlineStr">
         <is>
-          <t>1153 Dcc. 7.</t>
+          <t>1153 Dec. 7.</t>
         </is>
       </c>
       <c r="C1300" t="inlineStr">
@@ -41231,7 +41229,7 @@
       </c>
       <c r="B1301" t="inlineStr">
         <is>
-          <t>1153 Dcc. 7.</t>
+          <t>1153 Dec. 7.</t>
         </is>
       </c>
       <c r="C1301" t="inlineStr">
@@ -41263,7 +41261,7 @@
       </c>
       <c r="B1302" t="inlineStr">
         <is>
-          <t>1153 Dcc. 7.</t>
+          <t>1153 Dec. 7.</t>
         </is>
       </c>
       <c r="C1302" t="inlineStr">
@@ -42245,7 +42243,7 @@
       </c>
       <c r="D1333" t="inlineStr">
         <is>
-          <t>1153—</t>
+          <t>1153</t>
         </is>
       </c>
       <c r="E1333" t="inlineStr">
@@ -44031,7 +44029,7 @@
       </c>
       <c r="B1390" t="inlineStr">
         <is>
-          <t>1154 Agr. 25.</t>
+          <t>1154 Apr. 25.</t>
         </is>
       </c>
       <c r="C1390" t="inlineStr">
@@ -44063,7 +44061,7 @@
       </c>
       <c r="B1391" t="inlineStr">
         <is>
-          <t>1154 Agr. 6.</t>
+          <t>1154 Apr. 6.</t>
         </is>
       </c>
       <c r="C1391" t="inlineStr">
@@ -44095,7 +44093,7 @@
       </c>
       <c r="B1392" t="inlineStr">
         <is>
-          <t>1154 Agr. 8.</t>
+          <t>1154 Apr. 8.</t>
         </is>
       </c>
       <c r="C1392" t="inlineStr">
@@ -44933,7 +44931,7 @@
       </c>
       <c r="D1418" t="inlineStr">
         <is>
-          <t>9684:</t>
+          <t>9684</t>
         </is>
       </c>
       <c r="E1418" t="inlineStr">
@@ -45811,7 +45809,7 @@
       </c>
       <c r="B1446" t="inlineStr">
         <is>
-          <t>904 lun. 1.</t>
+          <t>904 Iun. 1.</t>
         </is>
       </c>
       <c r="C1446" t="inlineStr">
@@ -45843,7 +45841,7 @@
       </c>
       <c r="B1447" t="inlineStr">
         <is>
-          <t>904 lun. 4.</t>
+          <t>904 Iun. 4.</t>
         </is>
       </c>
       <c r="C1447" t="inlineStr">
@@ -45875,7 +45873,7 @@
       </c>
       <c r="B1448" t="inlineStr">
         <is>
-          <t>904 lun. 5.</t>
+          <t>904 Iun. 5.</t>
         </is>
       </c>
       <c r="C1448" t="inlineStr">
@@ -45907,7 +45905,7 @@
       </c>
       <c r="B1449" t="inlineStr">
         <is>
-          <t>904 lun. 9.</t>
+          <t>904 Iun. 9.</t>
         </is>
       </c>
       <c r="C1449" t="inlineStr">
@@ -45939,7 +45937,7 @@
       </c>
       <c r="B1450" t="inlineStr">
         <is>
-          <t>904 lun. 9.</t>
+          <t>904 Iun. 9.</t>
         </is>
       </c>
       <c r="C1450" t="inlineStr">
@@ -45971,7 +45969,7 @@
       </c>
       <c r="B1451" t="inlineStr">
         <is>
-          <t>904 lun. 11.</t>
+          <t>904 Iun. 11.</t>
         </is>
       </c>
       <c r="C1451" t="inlineStr">
@@ -46035,7 +46033,7 @@
       </c>
       <c r="B1453" t="inlineStr">
         <is>
-          <t>904 lun. 25.</t>
+          <t>904 Iun. 25.</t>
         </is>
       </c>
       <c r="C1453" t="inlineStr">
@@ -46067,7 +46065,7 @@
       </c>
       <c r="B1454" t="inlineStr">
         <is>
-          <t>904 lun. 26.</t>
+          <t>904 Iun. 26.</t>
         </is>
       </c>
       <c r="C1454" t="inlineStr">
@@ -46127,7 +46125,7 @@
       </c>
       <c r="B1456" t="inlineStr">
         <is>
-          <t>1154 lul. 3.</t>
+          <t>1154 Iul. 3.</t>
         </is>
       </c>
       <c r="C1456" t="inlineStr">
@@ -46351,7 +46349,7 @@
       </c>
       <c r="B1463" t="inlineStr">
         <is>
-          <t>1154 Xov. 16.</t>
+          <t>1154 Nov. 16.</t>
         </is>
       </c>
       <c r="C1463" t="inlineStr">
@@ -46383,7 +46381,7 @@
       </c>
       <c r="B1464" t="inlineStr">
         <is>
-          <t>1154 Xov. 17.</t>
+          <t>1154 Nov. 17.</t>
         </is>
       </c>
       <c r="C1464" t="inlineStr">
@@ -46415,7 +46413,7 @@
       </c>
       <c r="B1465" t="inlineStr">
         <is>
-          <t>1154 Xov. 17.</t>
+          <t>1154 Nov. 17.</t>
         </is>
       </c>
       <c r="C1465" t="inlineStr">
@@ -46447,7 +46445,7 @@
       </c>
       <c r="B1466" t="inlineStr">
         <is>
-          <t>1154 Xov. 19.</t>
+          <t>1154 Nov. 19.</t>
         </is>
       </c>
       <c r="C1466" t="inlineStr">
@@ -46479,7 +46477,7 @@
       </c>
       <c r="B1467" t="inlineStr">
         <is>
-          <t>1154 Xov. 21.</t>
+          <t>1154 Nov. 21.</t>
         </is>
       </c>
       <c r="C1467" t="inlineStr">
@@ -46511,7 +46509,7 @@
       </c>
       <c r="B1468" t="inlineStr">
         <is>
-          <t>1154 Xov. 28.</t>
+          <t>1154 Nov. 28.</t>
         </is>
       </c>
       <c r="C1468" t="inlineStr">
@@ -46543,7 +46541,7 @@
       </c>
       <c r="B1469" t="inlineStr">
         <is>
-          <t>1154 Xov. 28.</t>
+          <t>1154 Nov. 28.</t>
         </is>
       </c>
       <c r="C1469" t="inlineStr">
@@ -49973,7 +49971,7 @@
       </c>
       <c r="D1579" t="inlineStr">
         <is>
-          <t>p10044</t>
+          <t>10044</t>
         </is>
       </c>
       <c r="E1579" t="inlineStr">
@@ -50023,7 +50021,7 @@
       </c>
       <c r="B1581" t="inlineStr">
         <is>
-          <t>1155 Nai. 1.</t>
+          <t>1155 Mai. 1.</t>
         </is>
       </c>
       <c r="C1581" t="inlineStr">
@@ -50051,7 +50049,7 @@
       </c>
       <c r="B1582" t="inlineStr">
         <is>
-          <t>1155 Nai. 2.</t>
+          <t>1155 Mai. 2.</t>
         </is>
       </c>
       <c r="C1582" t="inlineStr">
@@ -50083,7 +50081,7 @@
       </c>
       <c r="B1583" t="inlineStr">
         <is>
-          <t>1155 Nai. 2.</t>
+          <t>1155 Mai. 2.</t>
         </is>
       </c>
       <c r="C1583" t="inlineStr">
@@ -50115,7 +50113,7 @@
       </c>
       <c r="B1584" t="inlineStr">
         <is>
-          <t>1155 Nai. 4.</t>
+          <t>1155 Mai. 4.</t>
         </is>
       </c>
       <c r="C1584" t="inlineStr">
@@ -50143,7 +50141,7 @@
       </c>
       <c r="B1585" t="inlineStr">
         <is>
-          <t>1155 Nai. 6.</t>
+          <t>1155 Mai. 6.</t>
         </is>
       </c>
       <c r="C1585" t="inlineStr">
@@ -50175,7 +50173,7 @@
       </c>
       <c r="B1586" t="inlineStr">
         <is>
-          <t>1155 Nai. 6.</t>
+          <t>1155 Mai. 6.</t>
         </is>
       </c>
       <c r="C1586" t="inlineStr">
@@ -50207,7 +50205,7 @@
       </c>
       <c r="B1587" t="inlineStr">
         <is>
-          <t>1155 Nai. 7.</t>
+          <t>1155 Mai. 7.</t>
         </is>
       </c>
       <c r="C1587" t="inlineStr">
@@ -50239,7 +50237,7 @@
       </c>
       <c r="B1588" t="inlineStr">
         <is>
-          <t>1155 Nai. 7.</t>
+          <t>1155 Mai. 7.</t>
         </is>
       </c>
       <c r="C1588" t="inlineStr">
@@ -50271,7 +50269,7 @@
       </c>
       <c r="B1589" t="inlineStr">
         <is>
-          <t>1155 Nai. 9.</t>
+          <t>1155 Mai. 9.</t>
         </is>
       </c>
       <c r="C1589" t="inlineStr">
@@ -50303,7 +50301,7 @@
       </c>
       <c r="B1590" t="inlineStr">
         <is>
-          <t>1155 Nai. 10.</t>
+          <t>1155 Mai. 10.</t>
         </is>
       </c>
       <c r="C1590" t="inlineStr">
@@ -51227,7 +51225,7 @@
       </c>
       <c r="B1620" t="inlineStr">
         <is>
-          <t>1155 lun. 19.</t>
+          <t>1155 Iun. 19.</t>
         </is>
       </c>
       <c r="C1620" t="inlineStr">
@@ -51613,7 +51611,7 @@
       </c>
       <c r="D1634" t="inlineStr">
         <is>
-          <t>10085 0.</t>
+          <t>10085 0</t>
         </is>
       </c>
       <c r="E1634" t="inlineStr">
@@ -52513,7 +52511,7 @@
       </c>
       <c r="D1664" t="inlineStr">
         <is>
-          <t>10111a</t>
+          <t>10111</t>
         </is>
       </c>
       <c r="E1664" t="inlineStr">
@@ -52775,7 +52773,7 @@
       </c>
       <c r="B1673" t="inlineStr">
         <is>
-          <t>1156 Lan. 2.</t>
+          <t>1156 Ian. 2.</t>
         </is>
       </c>
       <c r="C1673" t="inlineStr">
@@ -52803,7 +52801,7 @@
       </c>
       <c r="B1674" t="inlineStr">
         <is>
-          <t>1156 Lan. 5.</t>
+          <t>1156 Ian. 5.</t>
         </is>
       </c>
       <c r="C1674" t="inlineStr">
@@ -52835,7 +52833,7 @@
       </c>
       <c r="B1675" t="inlineStr">
         <is>
-          <t>1156 Lan. 11.</t>
+          <t>1156 Ian. 11.</t>
         </is>
       </c>
       <c r="C1675" t="inlineStr">
@@ -52867,7 +52865,7 @@
       </c>
       <c r="B1676" t="inlineStr">
         <is>
-          <t>1156 Lan. 13.</t>
+          <t>1156 Ian. 13.</t>
         </is>
       </c>
       <c r="C1676" t="inlineStr">
@@ -52899,7 +52897,7 @@
       </c>
       <c r="B1677" t="inlineStr">
         <is>
-          <t>1156 Lan. 13.</t>
+          <t>1156 Ian. 13.</t>
         </is>
       </c>
       <c r="C1677" t="inlineStr">
@@ -52931,7 +52929,7 @@
       </c>
       <c r="B1678" t="inlineStr">
         <is>
-          <t>1156 Lan. 19.</t>
+          <t>1156 Ian. 19.</t>
         </is>
       </c>
       <c r="C1678" t="inlineStr">
@@ -52963,7 +52961,7 @@
       </c>
       <c r="B1679" t="inlineStr">
         <is>
-          <t>1156 Lan. 20.</t>
+          <t>1156 Ian. 20.</t>
         </is>
       </c>
       <c r="C1679" t="inlineStr">
@@ -52995,7 +52993,7 @@
       </c>
       <c r="B1680" t="inlineStr">
         <is>
-          <t>1156 Lan. 23.</t>
+          <t>1156 Ian. 23.</t>
         </is>
       </c>
       <c r="C1680" t="inlineStr">
@@ -53027,7 +53025,7 @@
       </c>
       <c r="B1681" t="inlineStr">
         <is>
-          <t>1156 Lan. 23.</t>
+          <t>1156 Ian. 23.</t>
         </is>
       </c>
       <c r="C1681" t="inlineStr">
@@ -53059,7 +53057,7 @@
       </c>
       <c r="B1682" t="inlineStr">
         <is>
-          <t>1156 Lan. 23.</t>
+          <t>1156 Ian. 23.</t>
         </is>
       </c>
       <c r="C1682" t="inlineStr">
@@ -53091,7 +53089,7 @@
       </c>
       <c r="B1683" t="inlineStr">
         <is>
-          <t>1156 Lan. 25.</t>
+          <t>1156 Ian. 25.</t>
         </is>
       </c>
       <c r="C1683" t="inlineStr">
@@ -53123,7 +53121,7 @@
       </c>
       <c r="B1684" t="inlineStr">
         <is>
-          <t>1156 Lan. 25.</t>
+          <t>1156 Ian. 25.</t>
         </is>
       </c>
       <c r="C1684" t="inlineStr">
@@ -53155,7 +53153,7 @@
       </c>
       <c r="B1685" t="inlineStr">
         <is>
-          <t>1156 Lan. 27.</t>
+          <t>1156 Ian. 27.</t>
         </is>
       </c>
       <c r="C1685" t="inlineStr">
@@ -53187,7 +53185,7 @@
       </c>
       <c r="B1686" t="inlineStr">
         <is>
-          <t>1156 Lan. 27.</t>
+          <t>1156 Ian. 27.</t>
         </is>
       </c>
       <c r="C1686" t="inlineStr">
@@ -54117,7 +54115,7 @@
       </c>
       <c r="D1715" t="inlineStr">
         <is>
-          <t>f 10163</t>
+          <t xml:space="preserve"> 10163</t>
         </is>
       </c>
       <c r="E1715" t="inlineStr">
@@ -54683,7 +54681,7 @@
       </c>
       <c r="B1733" t="inlineStr">
         <is>
-          <t>1156 lun. 1.</t>
+          <t>1156 Iun. 1.</t>
         </is>
       </c>
       <c r="C1733" t="inlineStr">
@@ -54715,7 +54713,7 @@
       </c>
       <c r="B1734" t="inlineStr">
         <is>
-          <t>1156 lun. 1.</t>
+          <t>1156 Iun. 1.</t>
         </is>
       </c>
       <c r="C1734" t="inlineStr">
@@ -54747,7 +54745,7 @@
       </c>
       <c r="B1735" t="inlineStr">
         <is>
-          <t>1156 lun. 6.</t>
+          <t>1156 Iun. 6.</t>
         </is>
       </c>
       <c r="C1735" t="inlineStr">
@@ -54779,7 +54777,7 @@
       </c>
       <c r="B1736" t="inlineStr">
         <is>
-          <t>1156 lun. 7.</t>
+          <t>1156 Iun. 7.</t>
         </is>
       </c>
       <c r="C1736" t="inlineStr">
@@ -54811,7 +54809,7 @@
       </c>
       <c r="B1737" t="inlineStr">
         <is>
-          <t>1156 lun. 7.</t>
+          <t>1156 Iun. 7.</t>
         </is>
       </c>
       <c r="C1737" t="inlineStr">
@@ -54843,7 +54841,7 @@
       </c>
       <c r="B1738" t="inlineStr">
         <is>
-          <t>1156 lun. 8.</t>
+          <t>1156 Iun. 8.</t>
         </is>
       </c>
       <c r="C1738" t="inlineStr">
@@ -54875,7 +54873,7 @@
       </c>
       <c r="B1739" t="inlineStr">
         <is>
-          <t>1156 lun. 9.</t>
+          <t>1156 Iun. 9.</t>
         </is>
       </c>
       <c r="C1739" t="inlineStr">
@@ -54911,11 +54909,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D1740" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="D1740" t="inlineStr"/>
       <c r="E1740" t="inlineStr">
         <is>
           <t>„Apostolice sedis“.</t>
@@ -54931,7 +54925,7 @@
       </c>
       <c r="B1741" t="inlineStr">
         <is>
-          <t>1156 lun. 9.</t>
+          <t>1156 Iun. 9.</t>
         </is>
       </c>
       <c r="C1741" t="inlineStr">
@@ -54963,7 +54957,7 @@
       </c>
       <c r="B1742" t="inlineStr">
         <is>
-          <t>1156 lun. 9.</t>
+          <t>1156 Iun. 9.</t>
         </is>
       </c>
       <c r="C1742" t="inlineStr">
@@ -54995,7 +54989,7 @@
       </c>
       <c r="B1743" t="inlineStr">
         <is>
-          <t>1156 lun. 11.</t>
+          <t>1156 Iun. 11.</t>
         </is>
       </c>
       <c r="C1743" t="inlineStr">
@@ -55005,7 +54999,7 @@
       </c>
       <c r="D1743" t="inlineStr">
         <is>
-          <t>10189a</t>
+          <t>10189</t>
         </is>
       </c>
       <c r="E1743" t="inlineStr">
@@ -55091,7 +55085,7 @@
       </c>
       <c r="B1746" t="inlineStr">
         <is>
-          <t>1156 lun. 18.</t>
+          <t>1156 Iun. 18.</t>
         </is>
       </c>
       <c r="C1746" t="inlineStr">
@@ -55183,7 +55177,7 @@
       </c>
       <c r="B1749" t="inlineStr">
         <is>
-          <t>1156 lul. 3.</t>
+          <t>1156 Iul. 3.</t>
         </is>
       </c>
       <c r="C1749" t="inlineStr">
@@ -55215,7 +55209,7 @@
       </c>
       <c r="B1750" t="inlineStr">
         <is>
-          <t>1156 lul. 3.</t>
+          <t>1156 Iul. 3.</t>
         </is>
       </c>
       <c r="C1750" t="inlineStr">
@@ -55279,7 +55273,7 @@
       </c>
       <c r="B1752" t="inlineStr">
         <is>
-          <t>1156 lul. 10.</t>
+          <t>1156 Iul. 10.</t>
         </is>
       </c>
       <c r="C1752" t="inlineStr">
@@ -56695,7 +56689,7 @@
       </c>
       <c r="B1798" t="inlineStr">
         <is>
-          <t>1157 lan. 4.</t>
+          <t>1157 Ian. 4.</t>
         </is>
       </c>
       <c r="C1798" t="inlineStr">
@@ -56727,7 +56721,7 @@
       </c>
       <c r="B1799" t="inlineStr">
         <is>
-          <t>1157 lan. 1.</t>
+          <t>1157 Ian. 1.</t>
         </is>
       </c>
       <c r="C1799" t="inlineStr">
@@ -56759,7 +56753,7 @@
       </c>
       <c r="B1800" t="inlineStr">
         <is>
-          <t>1157 lan. 1.</t>
+          <t>1157 Ian. 1.</t>
         </is>
       </c>
       <c r="C1800" t="inlineStr">
@@ -56791,7 +56785,7 @@
       </c>
       <c r="B1801" t="inlineStr">
         <is>
-          <t>1157 lan. 4.</t>
+          <t>1157 Ian. 4.</t>
         </is>
       </c>
       <c r="C1801" t="inlineStr">
@@ -56823,7 +56817,7 @@
       </c>
       <c r="B1802" t="inlineStr">
         <is>
-          <t>1157 lan. 13.</t>
+          <t>1157 Ian. 13.</t>
         </is>
       </c>
       <c r="C1802" t="inlineStr">
@@ -56855,7 +56849,7 @@
       </c>
       <c r="B1803" t="inlineStr">
         <is>
-          <t>1157 lan. 13.</t>
+          <t>1157 Ian. 13.</t>
         </is>
       </c>
       <c r="C1803" t="inlineStr">
@@ -56887,7 +56881,7 @@
       </c>
       <c r="B1804" t="inlineStr">
         <is>
-          <t>1157 lan. 19.</t>
+          <t>1157 Ian. 19.</t>
         </is>
       </c>
       <c r="C1804" t="inlineStr">
@@ -56919,7 +56913,7 @@
       </c>
       <c r="B1805" t="inlineStr">
         <is>
-          <t>1157 lan. 20.</t>
+          <t>1157 Ian. 20.</t>
         </is>
       </c>
       <c r="C1805" t="inlineStr">
@@ -58479,11 +58473,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="D1854" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
+      <c r="D1854" t="inlineStr"/>
       <c r="E1854" t="inlineStr">
         <is>
           <t>commendat. Nunciat, eidem ab (Lampridio) archiepiscopo Iadertino promissam obedientiam esse. Ughelli It. sacr. V. 1128, Mansi XXI. 825, Migne 188 p. 1520.</t>
@@ -58567,7 +58557,7 @@
       </c>
       <c r="B1857" t="inlineStr">
         <is>
-          <t>1157 Aor. 28.</t>
+          <t>1157 Apr. 28.</t>
         </is>
       </c>
       <c r="C1857" t="inlineStr">
@@ -58599,7 +58589,7 @@
       </c>
       <c r="B1858" t="inlineStr">
         <is>
-          <t>1030 Aor. 10.</t>
+          <t>1030 Apr. 10.</t>
         </is>
       </c>
       <c r="C1858" t="inlineStr">
@@ -59593,7 +59583,7 @@
       </c>
       <c r="D1889" t="inlineStr">
         <is>
-          <t>f10333</t>
+          <t>10333</t>
         </is>
       </c>
       <c r="E1889" t="inlineStr">
@@ -59625,7 +59615,7 @@
       </c>
       <c r="D1890" t="inlineStr">
         <is>
-          <t>p10334</t>
+          <t>10334</t>
         </is>
       </c>
       <c r="E1890" t="inlineStr">
@@ -60799,7 +60789,7 @@
       </c>
       <c r="B1927" t="inlineStr">
         <is>
-          <t>1157 lun. 11581.</t>
+          <t>1157 Iun. 11581.</t>
         </is>
       </c>
       <c r="C1927" t="inlineStr">
@@ -60831,7 +60821,7 @@
       </c>
       <c r="B1928" t="inlineStr">
         <is>
-          <t>1157 lun. 11581.</t>
+          <t>1157 Iun. 11581.</t>
         </is>
       </c>
       <c r="C1928" t="inlineStr">
@@ -60863,7 +60853,7 @@
       </c>
       <c r="B1929" t="inlineStr">
         <is>
-          <t>1157 Lun. 11581.</t>
+          <t>1157 Iun. 11581.</t>
         </is>
       </c>
       <c r="C1929" t="inlineStr">
@@ -60895,7 +60885,7 @@
       </c>
       <c r="B1930" t="inlineStr">
         <is>
-          <t>1157 Lun. 11584.</t>
+          <t>1157 Iun. 11584.</t>
         </is>
       </c>
       <c r="C1930" t="inlineStr">
@@ -60991,7 +60981,7 @@
       </c>
       <c r="B1933" t="inlineStr">
         <is>
-          <t>1158 lan. 3.</t>
+          <t>1158 Ian. 3.</t>
         </is>
       </c>
       <c r="C1933" t="inlineStr">
@@ -61055,7 +61045,7 @@
       </c>
       <c r="B1935" t="inlineStr">
         <is>
-          <t>1158 lan. 12.</t>
+          <t>1158 Ian. 12.</t>
         </is>
       </c>
       <c r="C1935" t="inlineStr">
@@ -61087,7 +61077,7 @@
       </c>
       <c r="B1936" t="inlineStr">
         <is>
-          <t>1158 lan. 21.</t>
+          <t>1158 Ian. 21.</t>
         </is>
       </c>
       <c r="C1936" t="inlineStr">
@@ -61119,7 +61109,7 @@
       </c>
       <c r="B1937" t="inlineStr">
         <is>
-          <t>1158 lan. 21.</t>
+          <t>1158 Ian. 21.</t>
         </is>
       </c>
       <c r="C1937" t="inlineStr">
@@ -61151,7 +61141,7 @@
       </c>
       <c r="B1938" t="inlineStr">
         <is>
-          <t>1158 lan. 22.</t>
+          <t>1158 Ian. 22.</t>
         </is>
       </c>
       <c r="C1938" t="inlineStr">
@@ -61183,7 +61173,7 @@
       </c>
       <c r="B1939" t="inlineStr">
         <is>
-          <t>1158 lan. 23.</t>
+          <t>1158 Ian. 23.</t>
         </is>
       </c>
       <c r="C1939" t="inlineStr">
@@ -61215,7 +61205,7 @@
       </c>
       <c r="B1940" t="inlineStr">
         <is>
-          <t>1158 lan. 25.</t>
+          <t>1158 Ian. 25.</t>
         </is>
       </c>
       <c r="C1940" t="inlineStr">
@@ -61247,7 +61237,7 @@
       </c>
       <c r="B1941" t="inlineStr">
         <is>
-          <t>1158 lan. 29.</t>
+          <t>1158 Ian. 29.</t>
         </is>
       </c>
       <c r="C1941" t="inlineStr">
@@ -61343,7 +61333,7 @@
       </c>
       <c r="B1944" t="inlineStr">
         <is>
-          <t>1158 lan. 15.</t>
+          <t>1158 Ian. 15.</t>
         </is>
       </c>
       <c r="C1944" t="inlineStr">
@@ -61375,7 +61365,7 @@
       </c>
       <c r="B1945" t="inlineStr">
         <is>
-          <t>1158 lan. 27.</t>
+          <t>1158 Ian. 27.</t>
         </is>
       </c>
       <c r="C1945" t="inlineStr">
@@ -61417,7 +61407,7 @@
       </c>
       <c r="D1946" t="inlineStr">
         <is>
-          <t>10389a</t>
+          <t>10389</t>
         </is>
       </c>
       <c r="E1946" t="inlineStr">
@@ -61911,7 +61901,7 @@
       </c>
       <c r="B1962" t="inlineStr">
         <is>
-          <t>1158 Nai. 10.</t>
+          <t>1158 Mai. 10.</t>
         </is>
       </c>
       <c r="C1962" t="inlineStr">
@@ -61943,7 +61933,7 @@
       </c>
       <c r="B1963" t="inlineStr">
         <is>
-          <t>1158 Nai. 11.</t>
+          <t>1158 Mai. 11.</t>
         </is>
       </c>
       <c r="C1963" t="inlineStr">
@@ -61975,7 +61965,7 @@
       </c>
       <c r="B1964" t="inlineStr">
         <is>
-          <t>1158 Nai. 14.</t>
+          <t>1158 Mai. 14.</t>
         </is>
       </c>
       <c r="C1964" t="inlineStr">
@@ -62007,7 +61997,7 @@
       </c>
       <c r="B1965" t="inlineStr">
         <is>
-          <t>1158 Nai. 16.</t>
+          <t>1158 Mai. 16.</t>
         </is>
       </c>
       <c r="C1965" t="inlineStr">
@@ -62039,7 +62029,7 @@
       </c>
       <c r="B1966" t="inlineStr">
         <is>
-          <t>1158 Nai. 20.</t>
+          <t>1158 Mai. 20.</t>
         </is>
       </c>
       <c r="C1966" t="inlineStr">
@@ -62387,7 +62377,7 @@
       </c>
       <c r="B1977" t="inlineStr">
         <is>
-          <t>1158 lun. 26.</t>
+          <t>1158 Iun. 26.</t>
         </is>
       </c>
       <c r="C1977" t="inlineStr">
@@ -62397,7 +62387,7 @@
       </c>
       <c r="D1977" t="inlineStr">
         <is>
-          <t>f10421</t>
+          <t>10421</t>
         </is>
       </c>
       <c r="E1977" t="inlineStr">
@@ -62419,7 +62409,7 @@
       </c>
       <c r="B1978" t="inlineStr">
         <is>
-          <t>1158 lul. 26.</t>
+          <t>1158 Iul. 26.</t>
         </is>
       </c>
       <c r="C1978" t="inlineStr">
@@ -62483,7 +62473,7 @@
       </c>
       <c r="B1980" t="inlineStr">
         <is>
-          <t>1158 lul. 19.</t>
+          <t>1158 Iul. 19.</t>
         </is>
       </c>
       <c r="C1980" t="inlineStr">
@@ -62597,7 +62587,7 @@
       </c>
       <c r="D1984" t="inlineStr">
         <is>
-          <t>f10425</t>
+          <t>10425</t>
         </is>
       </c>
       <c r="E1984" t="inlineStr">
@@ -63169,7 +63159,7 @@
       </c>
       <c r="D2002" t="inlineStr">
         <is>
-          <t>10443 (7065a</t>
+          <t>10443 (7065</t>
         </is>
       </c>
       <c r="E2002" t="inlineStr">
@@ -63795,7 +63785,7 @@
       </c>
       <c r="B2022" t="inlineStr">
         <is>
-          <t>1155 Iui. 11596.</t>
+          <t>1155 Iun. 11596.</t>
         </is>
       </c>
       <c r="C2022" t="inlineStr">
@@ -64019,7 +64009,7 @@
       </c>
       <c r="B2029" t="inlineStr">
         <is>
-          <t>1157 Lan. 11594.</t>
+          <t>1157 Ian. 11594.</t>
         </is>
       </c>
       <c r="C2029" t="inlineStr">
@@ -64051,7 +64041,7 @@
       </c>
       <c r="B2030" t="inlineStr">
         <is>
-          <t>1157 Lan. 11599.</t>
+          <t>1157 Ian. 11599.</t>
         </is>
       </c>
       <c r="C2030" t="inlineStr">
@@ -64083,7 +64073,7 @@
       </c>
       <c r="B2031" t="inlineStr">
         <is>
-          <t>1157 Lan. 115918.</t>
+          <t>1157 Ian. 115918.</t>
         </is>
       </c>
       <c r="C2031" t="inlineStr">
@@ -64115,7 +64105,7 @@
       </c>
       <c r="B2032" t="inlineStr">
         <is>
-          <t>1157 Lan. 115921.</t>
+          <t>1157 Ian. 115921.</t>
         </is>
       </c>
       <c r="C2032" t="inlineStr">
@@ -65427,7 +65417,7 @@
       </c>
       <c r="B2073" t="inlineStr">
         <is>
-          <t>1157 Nai. 115927.</t>
+          <t>1157 Mai. 115927.</t>
         </is>
       </c>
       <c r="C2073" t="inlineStr">
@@ -65459,7 +65449,7 @@
       </c>
       <c r="B2074" t="inlineStr">
         <is>
-          <t>1157 Nai. 11597.</t>
+          <t>1157 Mai. 11597.</t>
         </is>
       </c>
       <c r="C2074" t="inlineStr">
@@ -65491,7 +65481,7 @@
       </c>
       <c r="B2075" t="inlineStr">
         <is>
-          <t>1157 Nai. 11599.</t>
+          <t>1157 Mai. 11599.</t>
         </is>
       </c>
       <c r="C2075" t="inlineStr">
@@ -65523,7 +65513,7 @@
       </c>
       <c r="B2076" t="inlineStr">
         <is>
-          <t>1157 Nai. 115910.</t>
+          <t>1157 Mai. 115910.</t>
         </is>
       </c>
       <c r="C2076" t="inlineStr">
@@ -65555,7 +65545,7 @@
       </c>
       <c r="B2077" t="inlineStr">
         <is>
-          <t>1157 Nai. 115911.</t>
+          <t>1157 Mai. 115911.</t>
         </is>
       </c>
       <c r="C2077" t="inlineStr">
@@ -65587,7 +65577,7 @@
       </c>
       <c r="B2078" t="inlineStr">
         <is>
-          <t>1157 Nai. 115911.</t>
+          <t>1157 Mai. 115911.</t>
         </is>
       </c>
       <c r="C2078" t="inlineStr">
@@ -65619,7 +65609,7 @@
       </c>
       <c r="B2079" t="inlineStr">
         <is>
-          <t>1157 Nai. 115911.</t>
+          <t>1157 Mai. 115911.</t>
         </is>
       </c>
       <c r="C2079" t="inlineStr">
@@ -65651,7 +65641,7 @@
       </c>
       <c r="B2080" t="inlineStr">
         <is>
-          <t>1157 Nai. 115911.</t>
+          <t>1157 Mai. 115911.</t>
         </is>
       </c>
       <c r="C2080" t="inlineStr">
@@ -65683,7 +65673,7 @@
       </c>
       <c r="B2081" t="inlineStr">
         <is>
-          <t>1157 Nai. 115911.</t>
+          <t>1157 Mai. 115911.</t>
         </is>
       </c>
       <c r="C2081" t="inlineStr">
@@ -65715,7 +65705,7 @@
       </c>
       <c r="B2082" t="inlineStr">
         <is>
-          <t>1157 Nai. 115911.</t>
+          <t>1157 Mai. 115911.</t>
         </is>
       </c>
       <c r="C2082" t="inlineStr">
@@ -66191,7 +66181,7 @@
       </c>
       <c r="B2097" t="inlineStr">
         <is>
-          <t>1159 lan. 24.</t>
+          <t>1159 Ian. 24.</t>
         </is>
       </c>
       <c r="C2097" t="inlineStr">
@@ -66223,7 +66213,7 @@
       </c>
       <c r="B2098" t="inlineStr">
         <is>
-          <t>1159 lan. 29.</t>
+          <t>1159 Ian. 29.</t>
         </is>
       </c>
       <c r="C2098" t="inlineStr">
@@ -67259,7 +67249,7 @@
       </c>
       <c r="B2131" t="inlineStr">
         <is>
-          <t>1159 Noi. 27.</t>
+          <t>1159 Nov. 27.</t>
         </is>
       </c>
       <c r="C2131" t="inlineStr">
@@ -67291,7 +67281,7 @@
       </c>
       <c r="B2132" t="inlineStr">
         <is>
-          <t>1159 Noi. 30.</t>
+          <t>1159 Nov. 30.</t>
         </is>
       </c>
       <c r="C2132" t="inlineStr">
@@ -67323,7 +67313,7 @@
       </c>
       <c r="B2133" t="inlineStr">
         <is>
-          <t>1159 Noi. 30.</t>
+          <t>1159 Nov. 30.</t>
         </is>
       </c>
       <c r="C2133" t="inlineStr">
@@ -67355,7 +67345,7 @@
       </c>
       <c r="B2134" t="inlineStr">
         <is>
-          <t>1159 lun. 15.</t>
+          <t>1159 Iun. 15.</t>
         </is>
       </c>
       <c r="C2134" t="inlineStr">
@@ -67363,8 +67353,10 @@
           <t>Anagniae</t>
         </is>
       </c>
-      <c r="D2134" t="n">
-        <v>10574</v>
+      <c r="D2134" t="inlineStr">
+        <is>
+          <t>10574</t>
+        </is>
       </c>
       <c r="E2134" t="inlineStr">
         <is>
@@ -67381,7 +67373,7 @@
       </c>
       <c r="B2135" t="inlineStr">
         <is>
-          <t>1159 lun. 21.</t>
+          <t>1159 Iun. 21.</t>
         </is>
       </c>
       <c r="C2135" t="inlineStr">
@@ -67391,7 +67383,7 @@
       </c>
       <c r="D2135" t="inlineStr">
         <is>
-          <t>f10575 (7121)</t>
+          <t>10575 (7121)</t>
         </is>
       </c>
       <c r="E2135" t="inlineStr">
@@ -67413,7 +67405,7 @@
       </c>
       <c r="B2136" t="inlineStr">
         <is>
-          <t>1159 lun. 25.</t>
+          <t>1159 Iun. 25.</t>
         </is>
       </c>
       <c r="C2136" t="inlineStr">
@@ -67445,7 +67437,7 @@
       </c>
       <c r="B2137" t="inlineStr">
         <is>
-          <t>1159 lun. 28.</t>
+          <t>1159 Iun. 28.</t>
         </is>
       </c>
       <c r="C2137" t="inlineStr">
@@ -67477,7 +67469,7 @@
       </c>
       <c r="B2138" t="inlineStr">
         <is>
-          <t>1159 lun. 28.</t>
+          <t>1159 Iun. 28.</t>
         </is>
       </c>
       <c r="C2138" t="inlineStr">

</xml_diff>